<commit_message>
finish boms and cams
</commit_message>
<xml_diff>
--- a/mippe_mod/BOM_REV_A.xlsx
+++ b/mippe_mod/BOM_REV_A.xlsx
@@ -77,7 +77,7 @@
     <t xml:space="preserve">U2</t>
   </si>
   <si>
-    <t xml:space="preserve">QFN-44_EP_7.0x7.0x0.5P</t>
+    <t xml:space="preserve">TQFP-32_7.0x7.0x0.8P</t>
   </si>
   <si>
     <t xml:space="preserve">C14877</t>
@@ -401,7 +401,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>